<commit_message>
Add an entry with weird unicode values.
Fixes https://aptivate.kanbantool.com/b/437721-internews-hid-2018#20363239.
</commit_message>
<xml_diff>
--- a/internewshid/chn_spreadsheet/tests/test_files/sample_kobo.xlsx
+++ b/internewshid/chn_spreadsheet/tests/test_files/sample_kobo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t xml:space="preserve">start</t>
   </si>
@@ -119,6 +119,45 @@
   </si>
   <si>
     <t xml:space="preserve">2018-08-28T13:59:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-11T17:26:55.811+06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-11T17:29:09.865+06</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">tes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lohit Devanagari"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ရဂကငညဘလထအမ পরকত</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-11T17:27:00.000+06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kutupalong RC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">553c960d-3c2f-4349-a843-742cc9495dc8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-11T11:29:26</t>
   </si>
 </sst>
 </file>
@@ -128,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -150,6 +189,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lohit Devanagari"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -194,8 +239,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -216,10 +265,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40:M494"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -347,7 +396,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <v>27671657</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Configure Kobo importer to handle age range
</commit_message>
<xml_diff>
--- a/internewshid/chn_spreadsheet/tests/test_files/sample_kobo.xlsx
+++ b/internewshid/chn_spreadsheet/tests/test_files/sample_kobo.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">gender</t>
   </si>
   <si>
-    <t xml:space="preserve">Age</t>
+    <t xml:space="preserve">Age range</t>
   </si>
   <si>
     <t xml:space="preserve">Location</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">female</t>
   </si>
   <si>
-    <t xml:space="preserve">22</t>
+    <t xml:space="preserve">Age 19-25</t>
   </si>
   <si>
     <t xml:space="preserve">Camp 4</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">male</t>
   </si>
   <si>
-    <t xml:space="preserve">40</t>
+    <t xml:space="preserve">Age 36-45</t>
   </si>
   <si>
     <t xml:space="preserve">Camp 1W</t>
@@ -143,6 +143,7 @@
         <color rgb="FF000000"/>
         <rFont val="Lohit Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ရဂကငညဘလထအမ পরকত</t>
     </r>
@@ -195,6 +196,7 @@
       <color rgb="FF000000"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -268,10 +270,10 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>

</xml_diff>

<commit_message>
Update age range fixtures
Drop 'yrs' from categories
Change column to 'age' in importer configuration
</commit_message>
<xml_diff>
--- a/internewshid/chn_spreadsheet/tests/test_files/sample_kobo.xlsx
+++ b/internewshid/chn_spreadsheet/tests/test_files/sample_kobo.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">gender</t>
   </si>
   <si>
-    <t xml:space="preserve">Age range</t>
+    <t xml:space="preserve">age</t>
   </si>
   <si>
     <t xml:space="preserve">Location</t>
@@ -270,7 +270,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Fixed the spreadsheet test for risk
</commit_message>
<xml_diff>
--- a/internewshid/chn_spreadsheet/tests/test_files/sample_kobo.xlsx
+++ b/internewshid/chn_spreadsheet/tests/test_files/sample_kobo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t xml:space="preserve">start</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risk</t>
   </si>
   <si>
     <t xml:space="preserve">comment</t>
@@ -273,10 +276,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -327,130 +330,142 @@
       <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="J2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>27527921</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="M2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>29767031</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="M3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="true" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="1" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L4" s="1" t="n">
         <v>27671657</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="1" t="n">
+      <c r="N4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" s="1" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>